<commit_message>
Can now add individual articles
</commit_message>
<xml_diff>
--- a/src/Input/Sample Potch.xlsx
+++ b/src/Input/Sample Potch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
   <si>
     <t>Article</t>
   </si>
@@ -969,9 +969,6 @@
  Pag-aaralan din ng mga imbestigador ang maleta na mayroon pang price tag ng isang kilalang mall. Aalamin nila kung saang branch ng mall nabili ang maleta sa pag-asang makatulong ito para malutas ang krimen.
  Naghahanap din ang mga imbestigador ng closed-circuit-television camera sa lugar na posibleng nakakuha sa pag-iwan sa maleta.
  Dinala na ang bangkay ng babae sa Antipolo Funeral Homes sa Rizal. -- FRJ, GMA News</t>
-  </si>
-  <si>
-    <t>Chin chin</t>
   </si>
 </sst>
 </file>
@@ -1853,7 +1850,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" customHeight="1">

</xml_diff>